<commit_message>
doubled linked list were added!
</commit_message>
<xml_diff>
--- a/marks list.xlsx
+++ b/marks list.xlsx
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1148,14 +1148,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
-      <c r="A30">
+    <row r="30" spans="1:12" s="1" customFormat="1">
+      <c r="A30" s="1">
         <v>26</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1173,14 +1173,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
-      <c r="A32">
+    <row r="32" spans="1:12" s="1" customFormat="1">
+      <c r="A32" s="1">
         <v>28</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1394,14 +1394,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48">
+    <row r="48" spans="1:4" s="1" customFormat="1">
+      <c r="A48" s="1">
         <v>44</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="1" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1489,14 +1489,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
-      <c r="A55">
+    <row r="55" spans="1:4" s="1" customFormat="1">
+      <c r="A55" s="1">
         <v>51</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="1" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1598,14 +1598,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63">
+    <row r="63" spans="1:4" s="1" customFormat="1">
+      <c r="A63" s="1">
         <v>59</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1637,14 +1637,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66">
+    <row r="66" spans="1:4" s="1" customFormat="1">
+      <c r="A66" s="1">
         <v>62</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="1" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>